<commit_message>
refactor: Richmond VA Monthly/Annual reports added
</commit_message>
<xml_diff>
--- a/links.xlsx
+++ b/links.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Repositories\cares-allocation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Repositories\cares-act-allocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07504FB9-4F18-41AE-B651-133A4AD95B0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42853790-8339-4224-B6B3-BDA5B129B042}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3CB435B-C17C-411A-81B9-140E89A87919}"/>
   </bookViews>
@@ -36,41 +36,49 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>https://www.governor.virginia.gov/media/governorvirginiagov/secretary-of-finance/pdf/SOF--Memo-to-Localities---2nd-Round---07_28_20.pdf</t>
-  </si>
-  <si>
-    <t>https://home.treasury.gov/system/files/136/Interim-Report-of-Costs-by-Category-Incurred-by-State-and-Local-Recipients-through-June-30.pdf</t>
-  </si>
-  <si>
-    <t>https://home.treasury.gov/system/files/136/Census-Data-and-Methodology-Final.pdf</t>
-  </si>
-  <si>
-    <t>https://home.treasury.gov/system/files/136/Coronavirus-Relief-Fund-Guidance-for-State-Territorial-Local-and-Tribal-Governments.pdf</t>
-  </si>
-  <si>
-    <t>https://home.treasury.gov/system/files/136/Payments-to-States-and-Units-of-Local-Government.pdf</t>
-  </si>
-  <si>
-    <t>https://www.governor.virginia.gov/newsroom/all-releases/2020/july/headline-859682-en.html</t>
-  </si>
-  <si>
-    <t>http://hac.virginia.gov/documents/2020/Post-Session/Combined%20HAC%20Summary%20Document%207-27-20.pdf</t>
-  </si>
-  <si>
-    <t>https://www.finance.virginia.gov/media/governorvirginiagov/secretary-of-finance/pdf/SOF--Memo-to-Localities-5_12_20.pdf</t>
-  </si>
-  <si>
-    <t>https://www.virginia.gov/services/government/tax-and-finance/</t>
+    <t xml:space="preserve">https://www.governor.virginia.gov/media/governorvirginiagov/secretary-of-finance/pdf/SOF--Memo-to-Localities---2nd-Round---07_28_20.pdf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://home.treasury.gov/system/files/136/Interim-Report-of-Costs-by-Category-Incurred-by-State-and-Local-Recipients-through-June-30.pdf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://home.treasury.gov/system/files/136/Census-Data-and-Methodology-Final.pdf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://home.treasury.gov/system/files/136/Coronavirus-Relief-Fund-Guidance-for-State-Territorial-Local-and-Tribal-Governments.pdf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://home.treasury.gov/system/files/136/Payments-to-States-and-Units-of-Local-Government.pdf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.governor.virginia.gov/newsroom/all-releases/2020/july/headline-859682-en.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.finance.virginia.gov/media/governorvirginiagov/secretary-of-finance/pdf/SOF--Memo-to-Localities-5_12_20.pdf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hac.virginia.gov/documents/2020/Post-Session/Combined%20HAC%20Summary%20Document%207-27-20.pdf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.virginia.gov/services/government/tax-and-finance/ </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,13 +101,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -415,57 +426,68 @@
   <dimension ref="B2:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{1F59C94C-A573-476A-96FE-8A80C610E916}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{E49B3A82-39A2-4125-90A3-6C56EB108BFE}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{11D4AC33-4CD1-404B-AA49-84A48D18176A}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{CC32BEAE-D9C6-47C1-94A0-0FDAA829260C}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{084F8D60-42AC-4B78-BA76-24BE5C801FD9}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{82AEA49F-10B5-4BDD-9060-6C3FD9C66713}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{BF6A9B89-DED1-4E62-87B3-3129F16336ED}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{8D56F6AF-B329-4691-80B2-9B002317A907}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{45F32E47-2C5A-4BCC-8657-2501C19F683F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>